<commit_message>
fixed issues with denver and penn state not having a lat long
</commit_message>
<xml_diff>
--- a/NCAASchoolLatLong.xlsx
+++ b/NCAASchoolLatLong.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nels2\Documents\GitHub\ncaamhockeytransferportal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995C4E05-6135-426F-A349-5CE97FFDC031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E3C6EF-02DB-4241-ABDE-3241508E6005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Arizona State</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Penn State</t>
   </si>
 </sst>
 </file>
@@ -258,13 +264,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -546,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D67176D-1649-43BF-90C7-7BDBA608F0C3}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,463 +795,485 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B19">
-        <v>43.664400000000001</v>
+        <v>39.677999999999997</v>
       </c>
       <c r="C19">
-        <v>-85.478999999999999</v>
+        <v>-104.9614</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>42.377000000000002</v>
+        <v>43.664400000000001</v>
       </c>
       <c r="C20">
-        <v>-71.116699999999994</v>
+        <v>-85.478999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21">
-        <v>42.221499999999999</v>
+        <v>42.377000000000002</v>
       </c>
       <c r="C21">
-        <v>-71.799700000000001</v>
+        <v>-71.116699999999994</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22">
-        <v>46.495199999999997</v>
+        <v>42.221499999999999</v>
       </c>
       <c r="C22">
-        <v>-84.346699999999998</v>
+        <v>-71.799700000000001</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23">
-        <v>38.705800000000004</v>
+        <v>46.495199999999997</v>
       </c>
       <c r="C23">
-        <v>-90.491200000000006</v>
+        <v>-84.346699999999998</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24">
-        <v>40.785699999999999</v>
+        <v>38.705800000000004</v>
       </c>
       <c r="C24">
-        <v>-73.619</v>
+        <v>-90.491200000000006</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25">
-        <v>44.8643</v>
+        <v>40.785699999999999</v>
       </c>
       <c r="C25">
-        <v>-68.665700000000001</v>
+        <v>-73.619</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26">
-        <v>42.131100000000004</v>
+        <v>44.8643</v>
       </c>
       <c r="C26">
-        <v>-80.052000000000007</v>
+        <v>-68.665700000000001</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27">
-        <v>42.607399999999998</v>
+        <v>42.131100000000004</v>
       </c>
       <c r="C27">
-        <v>-71.157799999999995</v>
+        <v>-80.052000000000007</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28">
-        <v>39.508499999999998</v>
+        <v>42.607399999999998</v>
       </c>
       <c r="C28">
-        <v>-84.734800000000007</v>
+        <v>-71.157799999999995</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29">
-        <v>42.277999999999999</v>
+        <v>39.508499999999998</v>
       </c>
       <c r="C29">
-        <v>-83.738200000000006</v>
+        <v>-84.734800000000007</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30">
-        <v>42.729100000000003</v>
+        <v>42.277999999999999</v>
       </c>
       <c r="C30">
-        <v>-84.479399999999998</v>
+        <v>-83.738200000000006</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31">
+        <v>42.729100000000003</v>
+      </c>
+      <c r="C31">
+        <v>-84.479399999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>37</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>47.1691</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>-88.558300000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B33" s="1">
         <v>44.974699999999999</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C33" s="1">
         <v>-93.235399999999998</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33">
-        <v>46.812199999999997</v>
-      </c>
-      <c r="C33">
-        <v>-92.091300000000004</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="3">
-        <v>44.156500000000001</v>
-      </c>
-      <c r="C34" s="3">
-        <v>-93.992199999999997</v>
+        <v>38</v>
+      </c>
+      <c r="B34">
+        <v>46.812199999999997</v>
+      </c>
+      <c r="C34">
+        <v>-92.091300000000004</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="3">
-        <v>41.258299999999998</v>
-      </c>
-      <c r="C35" s="3">
-        <v>-96.012500000000003</v>
+        <v>39</v>
+      </c>
+      <c r="B35">
+        <v>44.156500000000001</v>
+      </c>
+      <c r="C35">
+        <v>-93.992199999999997</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="4">
-        <v>43.134765999999999</v>
-      </c>
-      <c r="C36" s="4">
-        <v>-70.935689999999994</v>
+        <v>40</v>
+      </c>
+      <c r="B36">
+        <v>41.258299999999998</v>
+      </c>
+      <c r="C36">
+        <v>-96.012500000000003</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B37" s="3">
-        <v>43.097000000000001</v>
+        <v>43.134765999999999</v>
       </c>
       <c r="C37" s="3">
-        <v>-79.035700000000006</v>
+        <v>-70.935689999999994</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="3">
-        <v>47.922800000000002</v>
-      </c>
-      <c r="C38" s="3">
-        <v>-97.061999999999998</v>
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>43.097000000000001</v>
+      </c>
+      <c r="C38">
+        <v>-79.035700000000006</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="3">
-        <v>42.338500000000003</v>
-      </c>
-      <c r="C39" s="3">
-        <v>-71.088800000000006</v>
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>47.922800000000002</v>
+      </c>
+      <c r="C39">
+        <v>-97.061999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="3">
-        <v>46.558</v>
-      </c>
-      <c r="C40" s="3">
-        <v>-87.404300000000006</v>
+        <v>43</v>
+      </c>
+      <c r="B40">
+        <v>42.338500000000003</v>
+      </c>
+      <c r="C40">
+        <v>-71.088800000000006</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="3">
-        <v>40.003900000000002</v>
-      </c>
-      <c r="C41" s="3">
-        <v>-83.018900000000002</v>
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>46.558</v>
+      </c>
+      <c r="C41">
+        <v>-87.404300000000006</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B42">
-        <v>40.345799999999997</v>
+        <v>40.003900000000002</v>
       </c>
       <c r="C42">
-        <v>-74.654899999999998</v>
+        <v>-83.018900000000002</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B43">
-        <v>41.825299999999999</v>
+        <v>40.798200000000001</v>
       </c>
       <c r="C43">
-        <v>-71.411600000000007</v>
+        <v>-77.855900000000005</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B44">
-        <v>41.4283</v>
+        <v>40.345799999999997</v>
       </c>
       <c r="C44">
-        <v>-72.872699999999995</v>
+        <v>-74.654899999999998</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45">
-        <v>43.085000000000001</v>
+        <v>41.825299999999999</v>
       </c>
       <c r="C45">
-        <v>-77.674899999999994</v>
+        <v>-71.411600000000007</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="B46">
-        <v>42.7303</v>
+        <v>41.4283</v>
       </c>
       <c r="C46">
-        <v>-73.676599999999993</v>
+        <v>-72.872699999999995</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B47">
-        <v>40.505000000000003</v>
+        <v>43.085000000000001</v>
       </c>
       <c r="C47">
-        <v>-80.147199999999998</v>
+        <v>-77.674899999999994</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B48">
-        <v>41.177199999999999</v>
+        <v>42.7303</v>
       </c>
       <c r="C48">
-        <v>-73.220100000000002</v>
+        <v>-73.676599999999993</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B49">
-        <v>45.556199999999997</v>
+        <v>40.505000000000003</v>
       </c>
       <c r="C49">
-        <v>-94.156999999999996</v>
+        <v>-80.147199999999998</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="B50">
-        <v>44.595999999999997</v>
+        <v>41.177199999999999</v>
       </c>
       <c r="C50">
-        <v>-75.143199999999993</v>
+        <v>-73.220100000000002</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="B51">
-        <v>44.9452</v>
+        <v>45.556199999999997</v>
       </c>
       <c r="C51">
-        <v>-93.169600000000003</v>
+        <v>-94.156999999999996</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="B52">
-        <v>42.067300000000003</v>
+        <v>44.595999999999997</v>
       </c>
       <c r="C52">
-        <v>-71.077200000000005</v>
+        <v>-75.143199999999993</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53">
-        <v>41.770899999999997</v>
+        <v>44.9452</v>
       </c>
       <c r="C53">
-        <v>-72.257300000000001</v>
+        <v>-93.169600000000003</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="B54">
-        <v>42.387900000000002</v>
+        <v>42.067300000000003</v>
       </c>
       <c r="C54">
-        <v>-72.528400000000005</v>
+        <v>-71.077200000000005</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B55">
-        <v>42.646500000000003</v>
+        <v>41.770899999999997</v>
       </c>
       <c r="C55">
-        <v>-71.321799999999996</v>
+        <v>-72.257300000000001</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B56">
-        <v>42.802100000000003</v>
+        <v>42.387900000000002</v>
       </c>
       <c r="C56">
-        <v>-73.939700000000002</v>
+        <v>-72.528400000000005</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B57">
-        <v>44.476399999999998</v>
+        <v>42.646500000000003</v>
       </c>
       <c r="C57">
-        <v>-73.193200000000004</v>
+        <v>-71.321799999999996</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B58" s="1">
-        <v>42.291699999999999</v>
-      </c>
-      <c r="C58" s="1">
-        <v>-85.587199999999996</v>
+      <c r="A58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58">
+        <v>42.802100000000003</v>
+      </c>
+      <c r="C58">
+        <v>-73.939700000000002</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59">
+        <v>44.476399999999998</v>
+      </c>
+      <c r="C59">
+        <v>-73.193200000000004</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="1">
+        <v>42.291699999999999</v>
+      </c>
+      <c r="C60" s="1">
+        <v>-85.587199999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>56</v>
       </c>
-      <c r="B59">
+      <c r="B61">
         <v>43.076300000000003</v>
       </c>
-      <c r="C59">
+      <c r="C61">
         <v>-89.403999999999996</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>57</v>
       </c>
-      <c r="B60">
+      <c r="B62">
         <v>41.311399999999999</v>
       </c>
-      <c r="C60">
+      <c r="C62">
         <v>-72.926400000000001</v>
       </c>
     </row>

</xml_diff>